<commit_message>
fix incorrect course code
</commit_message>
<xml_diff>
--- a/data/horarios.completos.raw.xlsx
+++ b/data/horarios.completos.raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121D2E87-3720-4887-8D04-4C7D57BDBA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEB74FD-3EB0-40E6-BB3C-4E51FD4AB8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="638" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3176" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3176" uniqueCount="711">
   <si>
     <t>UNIVERSIDAD NACIONAL MAYOR DE SAN MARCOS</t>
   </si>
@@ -2522,6 +2522,9 @@
   </si>
   <si>
     <t>MIÉRCOLES</t>
+  </si>
+  <si>
+    <t>C3S20814</t>
   </si>
 </sst>
 </file>
@@ -4085,8 +4088,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I190" sqref="I190"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B205" sqref="B205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11263,7 +11266,7 @@
         <v>405</v>
       </c>
       <c r="B205" s="202" t="s">
-        <v>103</v>
+        <v>710</v>
       </c>
       <c r="C205" s="206" t="s">
         <v>417</v>
@@ -14335,10 +14338,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:K21"/>
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14887,6 +14890,9 @@
       <c r="G22" s="112" t="s">
         <v>690</v>
       </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C30" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -18692,7 +18698,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:K28"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working on Monday schedules
</commit_message>
<xml_diff>
--- a/data/horarios.completos.raw.xlsx
+++ b/data/horarios.completos.raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813117B0-0F15-4D14-9CAE-D8A12891E959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199BE80B-9D6B-4BE3-8475-19E7CD954448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="638" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3766,16 +3766,16 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -4198,8 +4198,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O253"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G207" sqref="G207"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O108" sqref="A108:O108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,39 +4373,39 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="180" t="s">
-        <v>336</v>
-      </c>
-      <c r="B5" s="180" t="s">
-        <v>364</v>
-      </c>
-      <c r="C5" s="181" t="s">
-        <v>365</v>
-      </c>
-      <c r="D5" s="182">
-        <v>2</v>
-      </c>
-      <c r="E5" s="182">
-        <v>3</v>
-      </c>
-      <c r="F5" s="182">
-        <v>3</v>
-      </c>
-      <c r="G5" s="183" t="s">
-        <v>657</v>
-      </c>
-      <c r="H5" s="180" t="s">
-        <v>105</v>
-      </c>
-      <c r="I5" s="180"/>
-      <c r="J5" s="180"/>
-      <c r="K5" s="180"/>
-      <c r="L5" s="180"/>
-      <c r="M5" s="180"/>
-      <c r="N5" s="180"/>
-      <c r="O5" s="180">
-        <v>1</v>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="149" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="153" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="149">
+        <v>2</v>
+      </c>
+      <c r="E5" s="149">
+        <v>3</v>
+      </c>
+      <c r="F5" s="149">
+        <v>4</v>
+      </c>
+      <c r="G5" s="155" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" s="151" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="151"/>
+      <c r="J5" s="151"/>
+      <c r="K5" s="151"/>
+      <c r="L5" s="151"/>
+      <c r="M5" s="151"/>
+      <c r="N5" s="151"/>
+      <c r="O5" s="151">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -7978,38 +7978,38 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="130" t="s">
-        <v>102</v>
-      </c>
-      <c r="B108" s="130" t="s">
-        <v>106</v>
-      </c>
-      <c r="C108" s="134" t="s">
-        <v>107</v>
-      </c>
-      <c r="D108" s="130">
-        <v>2</v>
-      </c>
-      <c r="E108" s="130">
-        <v>2</v>
-      </c>
-      <c r="F108" s="130">
-        <v>1</v>
-      </c>
-      <c r="G108" s="131" t="s">
-        <v>108</v>
-      </c>
-      <c r="H108" s="130" t="s">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" s="149" t="s">
+        <v>312</v>
+      </c>
+      <c r="B108" s="149" t="s">
+        <v>315</v>
+      </c>
+      <c r="C108" s="153" t="s">
+        <v>316</v>
+      </c>
+      <c r="D108" s="151">
+        <v>2</v>
+      </c>
+      <c r="E108" s="151">
+        <v>2</v>
+      </c>
+      <c r="F108" s="151">
+        <v>3</v>
+      </c>
+      <c r="G108" s="152" t="s">
+        <v>69</v>
+      </c>
+      <c r="H108" s="149" t="s">
         <v>105</v>
       </c>
-      <c r="I108" s="130"/>
-      <c r="J108" s="130"/>
-      <c r="K108" s="130"/>
-      <c r="L108" s="130"/>
-      <c r="M108" s="130"/>
-      <c r="N108" s="130"/>
-      <c r="O108" s="130">
+      <c r="I108" s="149"/>
+      <c r="J108" s="149"/>
+      <c r="K108" s="149"/>
+      <c r="L108" s="149"/>
+      <c r="M108" s="149"/>
+      <c r="N108" s="149"/>
+      <c r="O108" s="149">
         <v>2</v>
       </c>
     </row>
@@ -8048,38 +8048,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="130" t="s">
-        <v>102</v>
-      </c>
-      <c r="B110" s="130" t="s">
-        <v>112</v>
-      </c>
-      <c r="C110" s="134" t="s">
-        <v>113</v>
-      </c>
-      <c r="D110" s="130">
-        <v>2</v>
-      </c>
-      <c r="E110" s="130">
-        <v>2</v>
-      </c>
-      <c r="F110" s="130">
-        <v>1</v>
-      </c>
-      <c r="G110" s="131" t="s">
-        <v>114</v>
-      </c>
-      <c r="H110" s="130" t="s">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A110" s="141" t="s">
+        <v>336</v>
+      </c>
+      <c r="B110" s="141" t="s">
+        <v>353</v>
+      </c>
+      <c r="C110" s="135" t="s">
+        <v>78</v>
+      </c>
+      <c r="D110" s="138">
+        <v>2</v>
+      </c>
+      <c r="E110" s="138">
+        <v>2</v>
+      </c>
+      <c r="F110" s="138">
+        <v>2</v>
+      </c>
+      <c r="G110" s="142" t="s">
+        <v>289</v>
+      </c>
+      <c r="H110" s="141" t="s">
         <v>105</v>
       </c>
-      <c r="I110" s="130"/>
-      <c r="J110" s="130"/>
-      <c r="K110" s="130"/>
-      <c r="L110" s="130"/>
-      <c r="M110" s="130"/>
-      <c r="N110" s="130"/>
-      <c r="O110" s="130">
+      <c r="I110" s="141"/>
+      <c r="J110" s="141"/>
+      <c r="K110" s="141"/>
+      <c r="L110" s="141"/>
+      <c r="M110" s="141"/>
+      <c r="N110" s="141"/>
+      <c r="O110" s="141">
         <v>1</v>
       </c>
     </row>
@@ -8223,38 +8223,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="130" t="s">
-        <v>102</v>
-      </c>
-      <c r="B115" s="130" t="s">
-        <v>125</v>
-      </c>
-      <c r="C115" s="134" t="s">
-        <v>126</v>
-      </c>
-      <c r="D115" s="130">
-        <v>2</v>
-      </c>
-      <c r="E115" s="130">
-        <v>3</v>
-      </c>
-      <c r="F115" s="130">
-        <v>2</v>
-      </c>
-      <c r="G115" s="131" t="s">
-        <v>127</v>
-      </c>
-      <c r="H115" s="130" t="s">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" s="141" t="s">
+        <v>336</v>
+      </c>
+      <c r="B115" s="141" t="s">
+        <v>374</v>
+      </c>
+      <c r="C115" s="145" t="s">
+        <v>375</v>
+      </c>
+      <c r="D115" s="141">
+        <v>2</v>
+      </c>
+      <c r="E115" s="141">
+        <v>3</v>
+      </c>
+      <c r="F115" s="141">
+        <v>4</v>
+      </c>
+      <c r="G115" s="142" t="s">
+        <v>682</v>
+      </c>
+      <c r="H115" s="141" t="s">
         <v>105</v>
       </c>
-      <c r="I115" s="130"/>
-      <c r="J115" s="130"/>
-      <c r="K115" s="130"/>
-      <c r="L115" s="130"/>
-      <c r="M115" s="130"/>
-      <c r="N115" s="130"/>
-      <c r="O115" s="130">
+      <c r="I115" s="141"/>
+      <c r="J115" s="141"/>
+      <c r="K115" s="141"/>
+      <c r="L115" s="141"/>
+      <c r="M115" s="141"/>
+      <c r="N115" s="141"/>
+      <c r="O115" s="141">
         <v>1</v>
       </c>
     </row>
@@ -8398,38 +8398,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="130" t="s">
-        <v>102</v>
-      </c>
-      <c r="B120" s="130" t="s">
-        <v>556</v>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A120" s="140" t="s">
+        <v>151</v>
+      </c>
+      <c r="B120" s="140" t="s">
+        <v>560</v>
       </c>
       <c r="C120" s="134" t="s">
-        <v>138</v>
-      </c>
-      <c r="D120" s="130">
-        <v>2</v>
-      </c>
-      <c r="E120" s="130">
-        <v>3</v>
-      </c>
-      <c r="F120" s="130">
-        <v>3</v>
-      </c>
-      <c r="G120" s="131" t="s">
-        <v>96</v>
-      </c>
-      <c r="H120" s="130" t="s">
-        <v>105</v>
-      </c>
-      <c r="I120" s="130"/>
-      <c r="J120" s="130"/>
-      <c r="K120" s="130"/>
-      <c r="L120" s="130"/>
-      <c r="M120" s="130"/>
-      <c r="N120" s="130"/>
-      <c r="O120" s="130">
+        <v>181</v>
+      </c>
+      <c r="D120" s="140">
+        <v>2</v>
+      </c>
+      <c r="E120" s="140">
+        <v>3</v>
+      </c>
+      <c r="F120" s="140">
+        <v>3</v>
+      </c>
+      <c r="G120" s="144" t="s">
+        <v>165</v>
+      </c>
+      <c r="H120" s="140" t="s">
+        <v>175</v>
+      </c>
+      <c r="I120" s="140"/>
+      <c r="J120" s="140"/>
+      <c r="K120" s="140"/>
+      <c r="L120" s="140"/>
+      <c r="M120" s="140"/>
+      <c r="N120" s="140"/>
+      <c r="O120" s="140">
         <v>2</v>
       </c>
     </row>
@@ -8468,74 +8468,74 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="138" t="s">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A122" s="130" t="s">
+        <v>312</v>
+      </c>
+      <c r="B122" s="130" t="s">
+        <v>317</v>
+      </c>
+      <c r="C122" s="134" t="s">
+        <v>318</v>
+      </c>
+      <c r="D122" s="140">
+        <v>2</v>
+      </c>
+      <c r="E122" s="140">
+        <v>2</v>
+      </c>
+      <c r="F122" s="140">
+        <v>3</v>
+      </c>
+      <c r="G122" s="131" t="s">
+        <v>36</v>
+      </c>
+      <c r="H122" s="130" t="s">
+        <v>105</v>
+      </c>
+      <c r="I122" s="130"/>
+      <c r="J122" s="130"/>
+      <c r="K122" s="130"/>
+      <c r="L122" s="130"/>
+      <c r="M122" s="130"/>
+      <c r="N122" s="130"/>
+      <c r="O122" s="130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123" s="130" t="s">
         <v>102</v>
       </c>
-      <c r="B122" s="138" t="s">
-        <v>142</v>
-      </c>
-      <c r="C122" s="135" t="s">
-        <v>143</v>
-      </c>
-      <c r="D122" s="138">
-        <v>2</v>
-      </c>
-      <c r="E122" s="138">
-        <v>3</v>
-      </c>
-      <c r="F122" s="138">
-        <v>4</v>
-      </c>
-      <c r="G122" s="139" t="s">
-        <v>124</v>
-      </c>
-      <c r="H122" s="138" t="s">
+      <c r="B123" s="130" t="s">
+        <v>112</v>
+      </c>
+      <c r="C123" s="134" t="s">
+        <v>113</v>
+      </c>
+      <c r="D123" s="130">
+        <v>2</v>
+      </c>
+      <c r="E123" s="130">
+        <v>2</v>
+      </c>
+      <c r="F123" s="130">
+        <v>1</v>
+      </c>
+      <c r="G123" s="131" t="s">
+        <v>114</v>
+      </c>
+      <c r="H123" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="I122" s="138"/>
-      <c r="J122" s="138"/>
-      <c r="K122" s="138"/>
-      <c r="L122" s="138"/>
-      <c r="M122" s="138"/>
-      <c r="N122" s="138"/>
-      <c r="O122" s="138" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="138" t="s">
-        <v>102</v>
-      </c>
-      <c r="B123" s="138" t="s">
-        <v>144</v>
-      </c>
-      <c r="C123" s="135" t="s">
-        <v>145</v>
-      </c>
-      <c r="D123" s="138">
-        <v>2</v>
-      </c>
-      <c r="E123" s="138">
-        <v>3</v>
-      </c>
-      <c r="F123" s="138">
-        <v>4</v>
-      </c>
-      <c r="G123" s="139" t="s">
-        <v>146</v>
-      </c>
-      <c r="H123" s="138" t="s">
-        <v>105</v>
-      </c>
-      <c r="I123" s="138"/>
-      <c r="J123" s="138"/>
-      <c r="K123" s="138"/>
-      <c r="L123" s="138"/>
-      <c r="M123" s="138"/>
-      <c r="N123" s="138"/>
-      <c r="O123" s="138">
-        <v>2</v>
+      <c r="I123" s="130"/>
+      <c r="J123" s="130"/>
+      <c r="K123" s="130"/>
+      <c r="L123" s="130"/>
+      <c r="M123" s="130"/>
+      <c r="N123" s="130"/>
+      <c r="O123" s="130">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -8608,15 +8608,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="130" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="B126" s="140" t="s">
-        <v>157</v>
+        <v>564</v>
       </c>
       <c r="C126" s="134" t="s">
-        <v>158</v>
+        <v>217</v>
       </c>
       <c r="D126" s="130">
         <v>2</v>
@@ -8625,10 +8625,10 @@
         <v>2</v>
       </c>
       <c r="F126" s="130">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G126" s="144" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="H126" s="140" t="s">
         <v>105</v>
@@ -8643,15 +8643,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="130" t="s">
         <v>151</v>
       </c>
       <c r="B127" s="140" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C127" s="134" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D127" s="130">
         <v>2</v>
@@ -8663,7 +8663,7 @@
         <v>1</v>
       </c>
       <c r="G127" s="144" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H127" s="140" t="s">
         <v>105</v>
@@ -8675,7 +8675,7 @@
       <c r="M127" s="140"/>
       <c r="N127" s="140"/>
       <c r="O127" s="140">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -8783,15 +8783,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="130" t="s">
         <v>151</v>
       </c>
       <c r="B131" s="140" t="s">
-        <v>168</v>
+        <v>557</v>
       </c>
       <c r="C131" s="134" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="D131" s="130">
         <v>2</v>
@@ -8800,13 +8800,13 @@
         <v>3</v>
       </c>
       <c r="F131" s="130">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G131" s="144" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="H131" s="140" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="I131" s="140"/>
       <c r="J131" s="140"/>
@@ -8818,39 +8818,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="138" t="s">
-        <v>151</v>
-      </c>
-      <c r="B132" s="141" t="s">
-        <v>171</v>
-      </c>
-      <c r="C132" s="135" t="s">
-        <v>78</v>
-      </c>
-      <c r="D132" s="138">
-        <v>2</v>
-      </c>
-      <c r="E132" s="138">
-        <v>2</v>
-      </c>
-      <c r="F132" s="138">
-        <v>2</v>
-      </c>
-      <c r="G132" s="142" t="s">
-        <v>121</v>
-      </c>
-      <c r="H132" s="141" t="s">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A132" s="130" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132" s="130" t="s">
+        <v>207</v>
+      </c>
+      <c r="C132" s="134" t="s">
+        <v>208</v>
+      </c>
+      <c r="D132" s="130">
+        <v>2</v>
+      </c>
+      <c r="E132" s="130">
+        <v>2</v>
+      </c>
+      <c r="F132" s="130">
+        <v>2</v>
+      </c>
+      <c r="G132" s="131" t="s">
+        <v>616</v>
+      </c>
+      <c r="H132" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="I132" s="141"/>
-      <c r="J132" s="141"/>
-      <c r="K132" s="141"/>
-      <c r="L132" s="141"/>
-      <c r="M132" s="141"/>
-      <c r="N132" s="141"/>
-      <c r="O132" s="141">
-        <v>2</v>
+      <c r="I132" s="130"/>
+      <c r="J132" s="130"/>
+      <c r="K132" s="130"/>
+      <c r="L132" s="130"/>
+      <c r="M132" s="130"/>
+      <c r="N132" s="130"/>
+      <c r="O132" s="130">
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -8993,30 +8993,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="130" t="s">
-        <v>151</v>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A137" s="140" t="s">
+        <v>193</v>
       </c>
       <c r="B137" s="140" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="C137" s="134" t="s">
-        <v>178</v>
-      </c>
-      <c r="D137" s="130">
-        <v>2</v>
-      </c>
-      <c r="E137" s="130">
-        <v>3</v>
-      </c>
-      <c r="F137" s="130">
-        <v>3</v>
+        <v>213</v>
+      </c>
+      <c r="D137" s="140">
+        <v>2</v>
+      </c>
+      <c r="E137" s="140">
+        <v>2</v>
+      </c>
+      <c r="F137" s="140">
+        <v>2</v>
       </c>
       <c r="G137" s="144" t="s">
-        <v>159</v>
+        <v>618</v>
       </c>
       <c r="H137" s="140" t="s">
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="I137" s="140"/>
       <c r="J137" s="140"/>
@@ -9024,8 +9024,8 @@
       <c r="L137" s="140"/>
       <c r="M137" s="140"/>
       <c r="N137" s="140"/>
-      <c r="O137" s="140">
-        <v>1</v>
+      <c r="O137" s="140" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -9063,38 +9063,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="140" t="s">
-        <v>151</v>
-      </c>
-      <c r="B139" s="140" t="s">
-        <v>560</v>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A139" s="130" t="s">
+        <v>102</v>
+      </c>
+      <c r="B139" s="130" t="s">
+        <v>556</v>
       </c>
       <c r="C139" s="134" t="s">
-        <v>181</v>
-      </c>
-      <c r="D139" s="140">
-        <v>2</v>
-      </c>
-      <c r="E139" s="140">
-        <v>3</v>
-      </c>
-      <c r="F139" s="140">
-        <v>3</v>
-      </c>
-      <c r="G139" s="144" t="s">
-        <v>165</v>
-      </c>
-      <c r="H139" s="140" t="s">
-        <v>175</v>
-      </c>
-      <c r="I139" s="140"/>
-      <c r="J139" s="140"/>
-      <c r="K139" s="140"/>
-      <c r="L139" s="140"/>
-      <c r="M139" s="140"/>
-      <c r="N139" s="140"/>
-      <c r="O139" s="140">
+        <v>138</v>
+      </c>
+      <c r="D139" s="130">
+        <v>2</v>
+      </c>
+      <c r="E139" s="130">
+        <v>3</v>
+      </c>
+      <c r="F139" s="130">
+        <v>3</v>
+      </c>
+      <c r="G139" s="131" t="s">
+        <v>96</v>
+      </c>
+      <c r="H139" s="130" t="s">
+        <v>105</v>
+      </c>
+      <c r="I139" s="130"/>
+      <c r="J139" s="130"/>
+      <c r="K139" s="130"/>
+      <c r="L139" s="130"/>
+      <c r="M139" s="130"/>
+      <c r="N139" s="130"/>
+      <c r="O139" s="130">
         <v>2</v>
       </c>
     </row>
@@ -9133,74 +9133,74 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="138" t="s">
-        <v>151</v>
-      </c>
-      <c r="B141" s="141" t="s">
-        <v>184</v>
-      </c>
-      <c r="C141" s="135" t="s">
-        <v>185</v>
-      </c>
-      <c r="D141" s="138">
-        <v>2</v>
-      </c>
-      <c r="E141" s="138">
-        <v>2</v>
-      </c>
-      <c r="F141" s="138">
-        <v>4</v>
-      </c>
-      <c r="G141" s="142" t="s">
-        <v>186</v>
-      </c>
-      <c r="H141" s="141" t="s">
-        <v>175</v>
-      </c>
-      <c r="I141" s="141"/>
-      <c r="J141" s="141"/>
-      <c r="K141" s="141"/>
-      <c r="L141" s="141"/>
-      <c r="M141" s="141"/>
-      <c r="N141" s="141"/>
-      <c r="O141" s="141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="138" t="s">
-        <v>151</v>
-      </c>
-      <c r="B142" s="141" t="s">
-        <v>187</v>
-      </c>
-      <c r="C142" s="135" t="s">
-        <v>188</v>
-      </c>
-      <c r="D142" s="138">
-        <v>2</v>
-      </c>
-      <c r="E142" s="138">
-        <v>3</v>
-      </c>
-      <c r="F142" s="138">
-        <v>4</v>
-      </c>
-      <c r="G142" s="142" t="s">
-        <v>189</v>
-      </c>
-      <c r="H142" s="141" t="s">
-        <v>175</v>
-      </c>
-      <c r="I142" s="141"/>
-      <c r="J142" s="141"/>
-      <c r="K142" s="141"/>
-      <c r="L142" s="141"/>
-      <c r="M142" s="141"/>
-      <c r="N142" s="141"/>
-      <c r="O142" s="141">
-        <v>2</v>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A141" s="130" t="s">
+        <v>102</v>
+      </c>
+      <c r="B141" s="130" t="s">
+        <v>106</v>
+      </c>
+      <c r="C141" s="134" t="s">
+        <v>107</v>
+      </c>
+      <c r="D141" s="130">
+        <v>2</v>
+      </c>
+      <c r="E141" s="130">
+        <v>2</v>
+      </c>
+      <c r="F141" s="130">
+        <v>1</v>
+      </c>
+      <c r="G141" s="131" t="s">
+        <v>108</v>
+      </c>
+      <c r="H141" s="130" t="s">
+        <v>105</v>
+      </c>
+      <c r="I141" s="130"/>
+      <c r="J141" s="130"/>
+      <c r="K141" s="130"/>
+      <c r="L141" s="130"/>
+      <c r="M141" s="130"/>
+      <c r="N141" s="130"/>
+      <c r="O141" s="130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A142" s="130" t="s">
+        <v>193</v>
+      </c>
+      <c r="B142" s="130" t="s">
+        <v>202</v>
+      </c>
+      <c r="C142" s="134" t="s">
+        <v>203</v>
+      </c>
+      <c r="D142" s="130">
+        <v>2</v>
+      </c>
+      <c r="E142" s="130">
+        <v>3</v>
+      </c>
+      <c r="F142" s="130">
+        <v>1</v>
+      </c>
+      <c r="G142" s="131" t="s">
+        <v>108</v>
+      </c>
+      <c r="H142" s="130" t="s">
+        <v>105</v>
+      </c>
+      <c r="I142" s="130"/>
+      <c r="J142" s="130"/>
+      <c r="K142" s="130"/>
+      <c r="L142" s="130"/>
+      <c r="M142" s="130"/>
+      <c r="N142" s="130"/>
+      <c r="O142" s="130">
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -9308,74 +9308,74 @@
         <v>47</v>
       </c>
     </row>
-    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="140" t="s">
-        <v>193</v>
-      </c>
-      <c r="B146" s="140" t="s">
-        <v>200</v>
-      </c>
-      <c r="C146" s="134" t="s">
-        <v>201</v>
-      </c>
-      <c r="D146" s="140">
-        <v>2</v>
-      </c>
-      <c r="E146" s="140">
-        <v>2</v>
-      </c>
-      <c r="F146" s="140">
-        <v>1</v>
-      </c>
-      <c r="G146" s="144" t="s">
-        <v>127</v>
-      </c>
-      <c r="H146" s="140" t="s">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A146" s="138" t="s">
+        <v>151</v>
+      </c>
+      <c r="B146" s="141" t="s">
+        <v>171</v>
+      </c>
+      <c r="C146" s="135" t="s">
+        <v>78</v>
+      </c>
+      <c r="D146" s="138">
+        <v>2</v>
+      </c>
+      <c r="E146" s="138">
+        <v>2</v>
+      </c>
+      <c r="F146" s="138">
+        <v>2</v>
+      </c>
+      <c r="G146" s="142" t="s">
+        <v>121</v>
+      </c>
+      <c r="H146" s="141" t="s">
         <v>105</v>
       </c>
-      <c r="I146" s="140"/>
-      <c r="J146" s="140"/>
-      <c r="K146" s="140"/>
-      <c r="L146" s="140"/>
-      <c r="M146" s="140"/>
-      <c r="N146" s="140"/>
-      <c r="O146" s="140" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="130" t="s">
-        <v>193</v>
-      </c>
-      <c r="B147" s="130" t="s">
-        <v>202</v>
-      </c>
-      <c r="C147" s="134" t="s">
-        <v>203</v>
-      </c>
-      <c r="D147" s="130">
-        <v>2</v>
-      </c>
-      <c r="E147" s="130">
-        <v>3</v>
-      </c>
-      <c r="F147" s="130">
-        <v>1</v>
-      </c>
-      <c r="G147" s="131" t="s">
-        <v>108</v>
-      </c>
-      <c r="H147" s="130" t="s">
+      <c r="I146" s="141"/>
+      <c r="J146" s="141"/>
+      <c r="K146" s="141"/>
+      <c r="L146" s="141"/>
+      <c r="M146" s="141"/>
+      <c r="N146" s="141"/>
+      <c r="O146" s="141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A147" s="141" t="s">
+        <v>336</v>
+      </c>
+      <c r="B147" s="141" t="s">
+        <v>372</v>
+      </c>
+      <c r="C147" s="145" t="s">
+        <v>373</v>
+      </c>
+      <c r="D147" s="141">
+        <v>2</v>
+      </c>
+      <c r="E147" s="141">
+        <v>3</v>
+      </c>
+      <c r="F147" s="141">
+        <v>4</v>
+      </c>
+      <c r="G147" s="142" t="s">
+        <v>296</v>
+      </c>
+      <c r="H147" s="141" t="s">
         <v>105</v>
       </c>
-      <c r="I147" s="130"/>
-      <c r="J147" s="130"/>
-      <c r="K147" s="130"/>
-      <c r="L147" s="130"/>
-      <c r="M147" s="130"/>
-      <c r="N147" s="130"/>
-      <c r="O147" s="130">
-        <v>1</v>
+      <c r="I147" s="141"/>
+      <c r="J147" s="141"/>
+      <c r="K147" s="141"/>
+      <c r="L147" s="141"/>
+      <c r="M147" s="141"/>
+      <c r="N147" s="141"/>
+      <c r="O147" s="141">
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -9448,15 +9448,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="130" t="s">
-        <v>193</v>
-      </c>
-      <c r="B150" s="130" t="s">
-        <v>207</v>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A150" s="140" t="s">
+        <v>336</v>
+      </c>
+      <c r="B150" s="140" t="s">
+        <v>342</v>
       </c>
       <c r="C150" s="134" t="s">
-        <v>208</v>
+        <v>343</v>
       </c>
       <c r="D150" s="130">
         <v>2</v>
@@ -9465,22 +9465,22 @@
         <v>2</v>
       </c>
       <c r="F150" s="130">
-        <v>2</v>
-      </c>
-      <c r="G150" s="131" t="s">
-        <v>616</v>
-      </c>
-      <c r="H150" s="130" t="s">
+        <v>1</v>
+      </c>
+      <c r="G150" s="144" t="s">
+        <v>149</v>
+      </c>
+      <c r="H150" s="140" t="s">
         <v>105</v>
       </c>
-      <c r="I150" s="130"/>
-      <c r="J150" s="130"/>
-      <c r="K150" s="130"/>
-      <c r="L150" s="130"/>
-      <c r="M150" s="130"/>
-      <c r="N150" s="130"/>
-      <c r="O150" s="130">
-        <v>1</v>
+      <c r="I150" s="140"/>
+      <c r="J150" s="140"/>
+      <c r="K150" s="140"/>
+      <c r="L150" s="140"/>
+      <c r="M150" s="140"/>
+      <c r="N150" s="140"/>
+      <c r="O150" s="140">
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -9553,27 +9553,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="140" t="s">
-        <v>193</v>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A153" s="130" t="s">
+        <v>151</v>
       </c>
       <c r="B153" s="140" t="s">
-        <v>561</v>
+        <v>160</v>
       </c>
       <c r="C153" s="134" t="s">
-        <v>213</v>
-      </c>
-      <c r="D153" s="140">
-        <v>2</v>
-      </c>
-      <c r="E153" s="140">
-        <v>2</v>
-      </c>
-      <c r="F153" s="140">
-        <v>2</v>
+        <v>161</v>
+      </c>
+      <c r="D153" s="130">
+        <v>2</v>
+      </c>
+      <c r="E153" s="130">
+        <v>2</v>
+      </c>
+      <c r="F153" s="130">
+        <v>1</v>
       </c>
       <c r="G153" s="144" t="s">
-        <v>618</v>
+        <v>162</v>
       </c>
       <c r="H153" s="140" t="s">
         <v>105</v>
@@ -9584,8 +9584,8 @@
       <c r="L153" s="140"/>
       <c r="M153" s="140"/>
       <c r="N153" s="140"/>
-      <c r="O153" s="140" t="s">
-        <v>47</v>
+      <c r="O153" s="140">
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -9623,50 +9623,50 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="130" t="s">
-        <v>193</v>
-      </c>
-      <c r="B155" s="140" t="s">
-        <v>563</v>
-      </c>
-      <c r="C155" s="134" t="s">
-        <v>215</v>
-      </c>
-      <c r="D155" s="130">
-        <v>2</v>
-      </c>
-      <c r="E155" s="130">
-        <v>2</v>
-      </c>
-      <c r="F155" s="130">
-        <v>3</v>
-      </c>
-      <c r="G155" s="144" t="s">
-        <v>216</v>
-      </c>
-      <c r="H155" s="140" t="s">
-        <v>105</v>
-      </c>
-      <c r="I155" s="140"/>
-      <c r="J155" s="140"/>
-      <c r="K155" s="140"/>
-      <c r="L155" s="140"/>
-      <c r="M155" s="140"/>
-      <c r="N155" s="140"/>
-      <c r="O155" s="140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="130" t="s">
-        <v>193</v>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A155" s="138" t="s">
+        <v>151</v>
+      </c>
+      <c r="B155" s="141" t="s">
+        <v>184</v>
+      </c>
+      <c r="C155" s="135" t="s">
+        <v>185</v>
+      </c>
+      <c r="D155" s="138">
+        <v>2</v>
+      </c>
+      <c r="E155" s="138">
+        <v>2</v>
+      </c>
+      <c r="F155" s="138">
+        <v>4</v>
+      </c>
+      <c r="G155" s="142" t="s">
+        <v>186</v>
+      </c>
+      <c r="H155" s="141" t="s">
+        <v>175</v>
+      </c>
+      <c r="I155" s="141"/>
+      <c r="J155" s="141"/>
+      <c r="K155" s="141"/>
+      <c r="L155" s="141"/>
+      <c r="M155" s="141"/>
+      <c r="N155" s="141"/>
+      <c r="O155" s="141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A156" s="140" t="s">
+        <v>336</v>
       </c>
       <c r="B156" s="140" t="s">
-        <v>564</v>
+        <v>362</v>
       </c>
       <c r="C156" s="134" t="s">
-        <v>217</v>
+        <v>363</v>
       </c>
       <c r="D156" s="130">
         <v>2</v>
@@ -9678,7 +9678,7 @@
         <v>3</v>
       </c>
       <c r="G156" s="144" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="H156" s="140" t="s">
         <v>105</v>
@@ -9798,39 +9798,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="141" t="s">
-        <v>193</v>
-      </c>
-      <c r="B160" s="141" t="s">
-        <v>224</v>
-      </c>
-      <c r="C160" s="145" t="s">
-        <v>225</v>
-      </c>
-      <c r="D160" s="141">
-        <v>2</v>
-      </c>
-      <c r="E160" s="141">
-        <v>3</v>
-      </c>
-      <c r="F160" s="141">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A160" s="138" t="s">
+        <v>102</v>
+      </c>
+      <c r="B160" s="138" t="s">
+        <v>142</v>
+      </c>
+      <c r="C160" s="135" t="s">
+        <v>143</v>
+      </c>
+      <c r="D160" s="138">
+        <v>2</v>
+      </c>
+      <c r="E160" s="138">
+        <v>3</v>
+      </c>
+      <c r="F160" s="138">
         <v>4</v>
       </c>
-      <c r="G160" s="142" t="s">
-        <v>216</v>
-      </c>
-      <c r="H160" s="141" t="s">
+      <c r="G160" s="139" t="s">
+        <v>124</v>
+      </c>
+      <c r="H160" s="138" t="s">
         <v>105</v>
       </c>
-      <c r="I160" s="141"/>
-      <c r="J160" s="141"/>
-      <c r="K160" s="141"/>
-      <c r="L160" s="141"/>
-      <c r="M160" s="141"/>
-      <c r="N160" s="141"/>
-      <c r="O160" s="141" t="s">
-        <v>47</v>
+      <c r="I160" s="138"/>
+      <c r="J160" s="138"/>
+      <c r="K160" s="138"/>
+      <c r="L160" s="138"/>
+      <c r="M160" s="138"/>
+      <c r="N160" s="138"/>
+      <c r="O160" s="138" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -9868,74 +9868,74 @@
         <v>20</v>
       </c>
     </row>
-    <row r="162" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="130" t="s">
-        <v>312</v>
-      </c>
-      <c r="B162" s="130" t="s">
-        <v>315</v>
+        <v>193</v>
+      </c>
+      <c r="B162" s="140" t="s">
+        <v>563</v>
       </c>
       <c r="C162" s="134" t="s">
-        <v>316</v>
-      </c>
-      <c r="D162" s="140">
-        <v>2</v>
-      </c>
-      <c r="E162" s="140">
-        <v>2</v>
-      </c>
-      <c r="F162" s="140">
-        <v>3</v>
-      </c>
-      <c r="G162" s="131" t="s">
-        <v>69</v>
-      </c>
-      <c r="H162" s="130" t="s">
+        <v>215</v>
+      </c>
+      <c r="D162" s="130">
+        <v>2</v>
+      </c>
+      <c r="E162" s="130">
+        <v>2</v>
+      </c>
+      <c r="F162" s="130">
+        <v>3</v>
+      </c>
+      <c r="G162" s="144" t="s">
+        <v>216</v>
+      </c>
+      <c r="H162" s="140" t="s">
         <v>105</v>
       </c>
-      <c r="I162" s="130"/>
-      <c r="J162" s="130"/>
-      <c r="K162" s="130"/>
-      <c r="L162" s="130"/>
-      <c r="M162" s="130"/>
-      <c r="N162" s="130"/>
-      <c r="O162" s="130">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="130" t="s">
-        <v>312</v>
-      </c>
-      <c r="B163" s="130" t="s">
-        <v>317</v>
-      </c>
-      <c r="C163" s="134" t="s">
-        <v>318</v>
-      </c>
-      <c r="D163" s="140">
-        <v>2</v>
-      </c>
-      <c r="E163" s="140">
-        <v>2</v>
-      </c>
-      <c r="F163" s="140">
-        <v>3</v>
-      </c>
-      <c r="G163" s="131" t="s">
-        <v>36</v>
-      </c>
-      <c r="H163" s="130" t="s">
+      <c r="I162" s="140"/>
+      <c r="J162" s="140"/>
+      <c r="K162" s="140"/>
+      <c r="L162" s="140"/>
+      <c r="M162" s="140"/>
+      <c r="N162" s="140"/>
+      <c r="O162" s="140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A163" s="141" t="s">
+        <v>193</v>
+      </c>
+      <c r="B163" s="141" t="s">
+        <v>224</v>
+      </c>
+      <c r="C163" s="145" t="s">
+        <v>225</v>
+      </c>
+      <c r="D163" s="141">
+        <v>2</v>
+      </c>
+      <c r="E163" s="141">
+        <v>3</v>
+      </c>
+      <c r="F163" s="141">
+        <v>4</v>
+      </c>
+      <c r="G163" s="142" t="s">
+        <v>216</v>
+      </c>
+      <c r="H163" s="141" t="s">
         <v>105</v>
       </c>
-      <c r="I163" s="130"/>
-      <c r="J163" s="130"/>
-      <c r="K163" s="130"/>
-      <c r="L163" s="130"/>
-      <c r="M163" s="130"/>
-      <c r="N163" s="130"/>
-      <c r="O163" s="130">
-        <v>1</v>
+      <c r="I163" s="141"/>
+      <c r="J163" s="141"/>
+      <c r="K163" s="141"/>
+      <c r="L163" s="141"/>
+      <c r="M163" s="141"/>
+      <c r="N163" s="141"/>
+      <c r="O163" s="141" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -10043,39 +10043,39 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="141" t="s">
-        <v>312</v>
-      </c>
-      <c r="B167" s="141" t="s">
-        <v>326</v>
-      </c>
-      <c r="C167" s="146" t="s">
-        <v>327</v>
-      </c>
-      <c r="D167" s="141">
-        <v>2</v>
-      </c>
-      <c r="E167" s="141">
-        <v>3</v>
-      </c>
-      <c r="F167" s="141">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A167" s="138" t="s">
+        <v>102</v>
+      </c>
+      <c r="B167" s="138" t="s">
+        <v>144</v>
+      </c>
+      <c r="C167" s="135" t="s">
+        <v>145</v>
+      </c>
+      <c r="D167" s="138">
+        <v>2</v>
+      </c>
+      <c r="E167" s="138">
+        <v>3</v>
+      </c>
+      <c r="F167" s="138">
         <v>4</v>
       </c>
-      <c r="G167" s="142" t="s">
-        <v>328</v>
-      </c>
-      <c r="H167" s="141" t="s">
+      <c r="G167" s="139" t="s">
+        <v>146</v>
+      </c>
+      <c r="H167" s="138" t="s">
         <v>105</v>
       </c>
-      <c r="I167" s="141"/>
-      <c r="J167" s="141"/>
-      <c r="K167" s="141"/>
-      <c r="L167" s="141"/>
-      <c r="M167" s="141"/>
-      <c r="N167" s="141"/>
-      <c r="O167" s="141">
-        <v>1</v>
+      <c r="I167" s="138"/>
+      <c r="J167" s="138"/>
+      <c r="K167" s="138"/>
+      <c r="L167" s="138"/>
+      <c r="M167" s="138"/>
+      <c r="N167" s="138"/>
+      <c r="O167" s="138">
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -10253,27 +10253,27 @@
         <v>47</v>
       </c>
     </row>
-    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="140" t="s">
-        <v>336</v>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A173" s="130" t="s">
+        <v>151</v>
       </c>
       <c r="B173" s="140" t="s">
-        <v>342</v>
+        <v>168</v>
       </c>
       <c r="C173" s="134" t="s">
-        <v>343</v>
+        <v>169</v>
       </c>
       <c r="D173" s="130">
         <v>2</v>
       </c>
       <c r="E173" s="130">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F173" s="130">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G173" s="144" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="H173" s="140" t="s">
         <v>105</v>
@@ -10285,7 +10285,7 @@
       <c r="M173" s="140"/>
       <c r="N173" s="140"/>
       <c r="O173" s="140">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -10393,27 +10393,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" s="141" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="B177" s="141" t="s">
-        <v>353</v>
-      </c>
-      <c r="C177" s="135" t="s">
-        <v>78</v>
-      </c>
-      <c r="D177" s="138">
-        <v>2</v>
-      </c>
-      <c r="E177" s="138">
-        <v>2</v>
-      </c>
-      <c r="F177" s="138">
-        <v>2</v>
+        <v>326</v>
+      </c>
+      <c r="C177" s="146" t="s">
+        <v>327</v>
+      </c>
+      <c r="D177" s="141">
+        <v>2</v>
+      </c>
+      <c r="E177" s="141">
+        <v>3</v>
+      </c>
+      <c r="F177" s="141">
+        <v>4</v>
       </c>
       <c r="G177" s="142" t="s">
-        <v>289</v>
+        <v>328</v>
       </c>
       <c r="H177" s="141" t="s">
         <v>105</v>
@@ -10568,39 +10568,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="140" t="s">
-        <v>336</v>
-      </c>
-      <c r="B182" s="140" t="s">
-        <v>362</v>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A182" s="130" t="s">
+        <v>102</v>
+      </c>
+      <c r="B182" s="130" t="s">
+        <v>125</v>
       </c>
       <c r="C182" s="134" t="s">
-        <v>363</v>
+        <v>126</v>
       </c>
       <c r="D182" s="130">
         <v>2</v>
       </c>
       <c r="E182" s="130">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F182" s="130">
-        <v>3</v>
-      </c>
-      <c r="G182" s="144" t="s">
-        <v>186</v>
-      </c>
-      <c r="H182" s="140" t="s">
+        <v>2</v>
+      </c>
+      <c r="G182" s="131" t="s">
+        <v>127</v>
+      </c>
+      <c r="H182" s="130" t="s">
         <v>105</v>
       </c>
-      <c r="I182" s="140"/>
-      <c r="J182" s="140"/>
-      <c r="K182" s="140"/>
-      <c r="L182" s="140"/>
-      <c r="M182" s="140"/>
-      <c r="N182" s="140"/>
-      <c r="O182" s="140">
-        <v>2</v>
+      <c r="I182" s="130"/>
+      <c r="J182" s="130"/>
+      <c r="K182" s="130"/>
+      <c r="L182" s="130"/>
+      <c r="M182" s="130"/>
+      <c r="N182" s="130"/>
+      <c r="O182" s="130">
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -10743,77 +10743,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="141" t="s">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A187" s="140" t="s">
+        <v>193</v>
+      </c>
+      <c r="B187" s="140" t="s">
+        <v>200</v>
+      </c>
+      <c r="C187" s="134" t="s">
+        <v>201</v>
+      </c>
+      <c r="D187" s="140">
+        <v>2</v>
+      </c>
+      <c r="E187" s="140">
+        <v>2</v>
+      </c>
+      <c r="F187" s="140">
+        <v>1</v>
+      </c>
+      <c r="G187" s="144" t="s">
+        <v>127</v>
+      </c>
+      <c r="H187" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="I187" s="140"/>
+      <c r="J187" s="140"/>
+      <c r="K187" s="140"/>
+      <c r="L187" s="140"/>
+      <c r="M187" s="140"/>
+      <c r="N187" s="140"/>
+      <c r="O187" s="140" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A188" s="180" t="s">
         <v>336</v>
       </c>
-      <c r="B187" s="141" t="s">
-        <v>372</v>
-      </c>
-      <c r="C187" s="145" t="s">
-        <v>373</v>
-      </c>
-      <c r="D187" s="141">
-        <v>2</v>
-      </c>
-      <c r="E187" s="141">
-        <v>3</v>
-      </c>
-      <c r="F187" s="141">
-        <v>4</v>
-      </c>
-      <c r="G187" s="142" t="s">
-        <v>296</v>
-      </c>
-      <c r="H187" s="141" t="s">
+      <c r="B188" s="180" t="s">
+        <v>364</v>
+      </c>
+      <c r="C188" s="181" t="s">
+        <v>365</v>
+      </c>
+      <c r="D188" s="182">
+        <v>2</v>
+      </c>
+      <c r="E188" s="182">
+        <v>3</v>
+      </c>
+      <c r="F188" s="182">
+        <v>3</v>
+      </c>
+      <c r="G188" s="183" t="s">
+        <v>657</v>
+      </c>
+      <c r="H188" s="180" t="s">
         <v>105</v>
       </c>
-      <c r="I187" s="141"/>
-      <c r="J187" s="141"/>
-      <c r="K187" s="141"/>
-      <c r="L187" s="141"/>
-      <c r="M187" s="141"/>
-      <c r="N187" s="141"/>
-      <c r="O187" s="141">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="188" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="141" t="s">
-        <v>336</v>
-      </c>
-      <c r="B188" s="141" t="s">
-        <v>374</v>
-      </c>
-      <c r="C188" s="145" t="s">
-        <v>375</v>
-      </c>
-      <c r="D188" s="141">
-        <v>2</v>
-      </c>
-      <c r="E188" s="141">
-        <v>3</v>
-      </c>
-      <c r="F188" s="141">
-        <v>4</v>
-      </c>
-      <c r="G188" s="142" t="s">
-        <v>682</v>
-      </c>
-      <c r="H188" s="141" t="s">
-        <v>105</v>
-      </c>
-      <c r="I188" s="141"/>
-      <c r="J188" s="141"/>
-      <c r="K188" s="141"/>
-      <c r="L188" s="141"/>
-      <c r="M188" s="141"/>
-      <c r="N188" s="141"/>
-      <c r="O188" s="141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I188" s="180"/>
+      <c r="J188" s="180"/>
+      <c r="K188" s="180"/>
+      <c r="L188" s="180"/>
+      <c r="M188" s="180"/>
+      <c r="N188" s="180"/>
+      <c r="O188" s="180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="149" t="s">
         <v>435</v>
       </c>
@@ -10988,7 +10988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="151" t="s">
         <v>420</v>
       </c>
@@ -11023,7 +11023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="157" t="s">
         <v>435</v>
       </c>
@@ -11198,7 +11198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="157" t="s">
         <v>435</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="157" t="s">
         <v>405</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="157" t="s">
         <v>435</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="157" t="s">
         <v>405</v>
       </c>
@@ -11618,7 +11618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="149" t="s">
         <v>435</v>
       </c>
@@ -11793,7 +11793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="149" t="s">
         <v>420</v>
       </c>
@@ -12034,7 +12034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="149" t="s">
         <v>435</v>
       </c>
@@ -12069,17 +12069,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="182" t="s">
         <v>405</v>
       </c>
       <c r="B225" s="181" t="s">
         <v>607</v>
       </c>
-      <c r="C225" s="227" t="s">
+      <c r="C225" s="224" t="s">
         <v>403</v>
       </c>
-      <c r="D225" s="228">
+      <c r="D225" s="225">
         <v>4</v>
       </c>
       <c r="E225" s="182">
@@ -12104,7 +12104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="149" t="s">
         <v>405</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="157" t="s">
         <v>380</v>
       </c>
@@ -12314,7 +12314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="157" t="s">
         <v>380</v>
       </c>
@@ -12349,7 +12349,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="157" t="s">
         <v>380</v>
       </c>
@@ -13072,17 +13072,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O253" xr:uid="{19913135-E9D4-4501-ADC9-98BB6EF0FE1A}">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="13">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A189:O233">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:O188">
       <sortCondition ref="G1:G253"/>
     </sortState>
   </autoFilter>
@@ -13118,109 +13113,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="228" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="226"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="228"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="226" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="226"/>
-      <c r="I2" s="226"/>
-      <c r="J2" s="226"/>
-      <c r="K2" s="226"/>
+      <c r="A2" s="228" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="226"/>
+      <c r="A3" s="228" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="228"/>
+      <c r="J3" s="228"/>
+      <c r="K3" s="228"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="226" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="226"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="226"/>
-      <c r="I5" s="226"/>
-      <c r="J5" s="226"/>
-      <c r="K5" s="226"/>
+      <c r="A5" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="228"/>
+      <c r="F5" s="228"/>
+      <c r="G5" s="228"/>
+      <c r="H5" s="228"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="228"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="226" t="s">
+      <c r="A6" s="228" t="s">
         <v>335</v>
       </c>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="226"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="226"/>
-      <c r="K6" s="226"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="228"/>
+      <c r="I6" s="228"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="228"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -13937,109 +13932,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="228" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="226"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="228"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="226" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="226"/>
-      <c r="I2" s="226"/>
-      <c r="J2" s="226"/>
-      <c r="K2" s="226"/>
+      <c r="A2" s="228" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="226"/>
+      <c r="A3" s="228" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="228"/>
+      <c r="J3" s="228"/>
+      <c r="K3" s="228"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="226" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="226"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="226"/>
-      <c r="I5" s="226"/>
-      <c r="J5" s="226"/>
-      <c r="K5" s="226"/>
+      <c r="A5" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="228"/>
+      <c r="F5" s="228"/>
+      <c r="G5" s="228"/>
+      <c r="H5" s="228"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="228"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="226" t="s">
+      <c r="A6" s="228" t="s">
         <v>376</v>
       </c>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="226"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="226"/>
-      <c r="K6" s="226"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="228"/>
+      <c r="I6" s="228"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="228"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -14478,109 +14473,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="228" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="226"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="228"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="226" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="226"/>
-      <c r="I2" s="226"/>
-      <c r="J2" s="226"/>
-      <c r="K2" s="226"/>
+      <c r="A2" s="228" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="226"/>
+      <c r="A3" s="228" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="228"/>
+      <c r="J3" s="228"/>
+      <c r="K3" s="228"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="226" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="226"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="226"/>
-      <c r="I5" s="226"/>
-      <c r="J5" s="226"/>
-      <c r="K5" s="226"/>
+      <c r="A5" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="228"/>
+      <c r="F5" s="228"/>
+      <c r="G5" s="228"/>
+      <c r="H5" s="228"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="228"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="226" t="s">
+      <c r="A6" s="228" t="s">
         <v>404</v>
       </c>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="226"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="226"/>
-      <c r="K6" s="226"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="228"/>
+      <c r="I6" s="228"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="228"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
       <c r="L7" s="120"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -15055,109 +15050,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="228" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="226"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="228"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="226" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="226"/>
-      <c r="I2" s="226"/>
-      <c r="J2" s="226"/>
-      <c r="K2" s="226"/>
+      <c r="A2" s="228" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="226"/>
+      <c r="A3" s="228" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="228"/>
+      <c r="J3" s="228"/>
+      <c r="K3" s="228"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="226" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="226"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="226"/>
-      <c r="I5" s="226"/>
-      <c r="J5" s="226"/>
-      <c r="K5" s="226"/>
+      <c r="A5" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="228"/>
+      <c r="F5" s="228"/>
+      <c r="G5" s="228"/>
+      <c r="H5" s="228"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="228"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="226" t="s">
+      <c r="A6" s="228" t="s">
         <v>419</v>
       </c>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="226"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="226"/>
-      <c r="K6" s="226"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="228"/>
+      <c r="I6" s="228"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="228"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -15609,109 +15604,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="228" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="226"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="228"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="226" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="226"/>
-      <c r="I2" s="226"/>
-      <c r="J2" s="226"/>
-      <c r="K2" s="226"/>
+      <c r="A2" s="228" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="226"/>
+      <c r="A3" s="228" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="228"/>
+      <c r="J3" s="228"/>
+      <c r="K3" s="228"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="226" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="226"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="226"/>
-      <c r="I5" s="226"/>
-      <c r="J5" s="226"/>
-      <c r="K5" s="226"/>
+      <c r="A5" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="228"/>
+      <c r="F5" s="228"/>
+      <c r="G5" s="228"/>
+      <c r="H5" s="228"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="228"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="226" t="s">
+      <c r="A6" s="228" t="s">
         <v>434</v>
       </c>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="226"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="226"/>
-      <c r="K6" s="226"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="228"/>
+      <c r="I6" s="228"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="228"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -16240,95 +16235,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>451</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>534</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -16852,102 +16847,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
-      <c r="J1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
+      <c r="J2" s="226"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
+      <c r="J3" s="226"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
-      <c r="J5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
+      <c r="J5" s="226"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>492</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
-      <c r="J6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
+      <c r="J6" s="226"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>535</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -17505,95 +17500,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>641</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -18163,106 +18158,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="225"/>
-      <c r="B8" s="225"/>
-      <c r="C8" s="225"/>
-      <c r="D8" s="225"/>
-      <c r="E8" s="225"/>
-      <c r="F8" s="225"/>
-      <c r="G8" s="225"/>
-      <c r="H8" s="225"/>
-      <c r="I8" s="225"/>
+      <c r="A8" s="227"/>
+      <c r="B8" s="227"/>
+      <c r="C8" s="227"/>
+      <c r="D8" s="227"/>
+      <c r="E8" s="227"/>
+      <c r="F8" s="227"/>
+      <c r="G8" s="227"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="227"/>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -18836,109 +18831,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
-      <c r="J1" s="224"/>
-      <c r="K1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226"/>
+      <c r="K1" s="226"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
+      <c r="J3" s="226"/>
+      <c r="K3" s="226"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
-      <c r="J5" s="224"/>
-      <c r="K5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
+      <c r="J5" s="226"/>
+      <c r="K5" s="226"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
-      <c r="J6" s="224"/>
-      <c r="K6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
+      <c r="J6" s="226"/>
+      <c r="K6" s="226"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -19635,109 +19630,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
-      <c r="J1" s="224"/>
-      <c r="K1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226"/>
+      <c r="K1" s="226"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
+      <c r="J3" s="226"/>
+      <c r="K3" s="226"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
-      <c r="J5" s="224"/>
-      <c r="K5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
+      <c r="J5" s="226"/>
+      <c r="K5" s="226"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
-      <c r="J6" s="224"/>
-      <c r="K6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
+      <c r="J6" s="226"/>
+      <c r="K6" s="226"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -20458,109 +20453,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
-      <c r="J1" s="224"/>
-      <c r="K1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="226"/>
+      <c r="K1" s="226"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
+      <c r="J3" s="226"/>
+      <c r="K3" s="226"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
-      <c r="J5" s="224"/>
-      <c r="K5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
+      <c r="J5" s="226"/>
+      <c r="K5" s="226"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
-      <c r="J6" s="224"/>
-      <c r="K6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
+      <c r="J6" s="226"/>
+      <c r="K6" s="226"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -21803,95 +21798,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>533</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>226</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
       <c r="J7" s="120"/>
       <c r="K7" s="120"/>
     </row>
@@ -22801,96 +22796,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="226" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="224" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
+      <c r="A2" s="226" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="224" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
+      <c r="A3" s="226" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="226"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="226"/>
+      <c r="I3" s="226"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>533</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="224" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="224"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
+      <c r="A5" s="226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="226"/>
+      <c r="C5" s="226"/>
+      <c r="D5" s="226"/>
+      <c r="E5" s="226"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="226"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="226" t="s">
         <v>269</v>
       </c>
-      <c r="B6" s="224"/>
-      <c r="C6" s="224"/>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="224"/>
-      <c r="G6" s="224"/>
-      <c r="H6" s="224"/>
-      <c r="I6" s="224"/>
+      <c r="B6" s="226"/>
+      <c r="C6" s="226"/>
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="226"/>
+      <c r="G6" s="226"/>
+      <c r="H6" s="226"/>
+      <c r="I6" s="226"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -23652,124 +23647,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="228" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="226"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="228"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="226" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="226"/>
-      <c r="I2" s="226"/>
-      <c r="J2" s="226"/>
-      <c r="K2" s="226"/>
+      <c r="A2" s="228" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="226"/>
-      <c r="C3" s="226"/>
-      <c r="D3" s="226"/>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="226"/>
-      <c r="I3" s="226"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="226"/>
+      <c r="A3" s="228" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="228"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="228"/>
+      <c r="J3" s="228"/>
+      <c r="K3" s="228"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="224" t="s">
+      <c r="A4" s="226" t="s">
         <v>532</v>
       </c>
-      <c r="B4" s="224"/>
-      <c r="C4" s="224"/>
-      <c r="D4" s="224"/>
-      <c r="E4" s="224"/>
-      <c r="F4" s="224"/>
-      <c r="G4" s="224"/>
-      <c r="H4" s="224"/>
-      <c r="I4" s="224"/>
-      <c r="J4" s="224"/>
-      <c r="K4" s="224"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
+      <c r="E4" s="226"/>
+      <c r="F4" s="226"/>
+      <c r="G4" s="226"/>
+      <c r="H4" s="226"/>
+      <c r="I4" s="226"/>
+      <c r="J4" s="226"/>
+      <c r="K4" s="226"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="226" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="226"/>
-      <c r="G5" s="226"/>
-      <c r="H5" s="226"/>
-      <c r="I5" s="226"/>
-      <c r="J5" s="226"/>
-      <c r="K5" s="226"/>
+      <c r="A5" s="228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="228"/>
+      <c r="C5" s="228"/>
+      <c r="D5" s="228"/>
+      <c r="E5" s="228"/>
+      <c r="F5" s="228"/>
+      <c r="G5" s="228"/>
+      <c r="H5" s="228"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="228"/>
+      <c r="K5" s="228"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="226" t="s">
+      <c r="A6" s="228" t="s">
         <v>311</v>
       </c>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="226"/>
-      <c r="G6" s="226"/>
-      <c r="H6" s="226"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="226"/>
-      <c r="K6" s="226"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="228"/>
+      <c r="I6" s="228"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="228"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="226" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="224"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="224"/>
-      <c r="E7" s="224"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="226"/>
+      <c r="D7" s="226"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="226"/>
+      <c r="J7" s="226"/>
+      <c r="K7" s="226"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="224" t="s">
+      <c r="A8" s="226" t="s">
         <v>642</v>
       </c>
-      <c r="B8" s="224"/>
-      <c r="C8" s="224"/>
-      <c r="D8" s="224"/>
-      <c r="E8" s="224"/>
-      <c r="F8" s="224"/>
-      <c r="G8" s="224"/>
-      <c r="H8" s="224"/>
-      <c r="I8" s="224"/>
-      <c r="J8" s="224"/>
-      <c r="K8" s="224"/>
+      <c r="B8" s="226"/>
+      <c r="C8" s="226"/>
+      <c r="D8" s="226"/>
+      <c r="E8" s="226"/>
+      <c r="F8" s="226"/>
+      <c r="G8" s="226"/>
+      <c r="H8" s="226"/>
+      <c r="I8" s="226"/>
+      <c r="J8" s="226"/>
+      <c r="K8" s="226"/>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">

</xml_diff>